<commit_message>
Update results and train script with validation dataset
</commit_message>
<xml_diff>
--- a/Other/Saved_Results_3_hidden_space_test.xlsx
+++ b/Other/Saved_Results_3_hidden_space_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albi2\Documents\GitHub\Variational-Autoencoder-for-EEG-analysis\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A29D21-D8FD-43AA-A159-664ADDE7498D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3482A02-9309-4426-BEE1-4682E297E6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="32">
   <si>
     <t>Subject</t>
   </si>
@@ -120,6 +120,21 @@
   </si>
   <si>
     <t>Small hidden layer classifeir</t>
+  </si>
+  <si>
+    <t>Sigmoid as VAE last layer</t>
+  </si>
+  <si>
+    <t>Exponential LR Scheduler</t>
+  </si>
+  <si>
+    <t>Validation set used</t>
+  </si>
+  <si>
+    <t>Train for 500 epoch, exp lr scheduler, VERY BAD RESULTS</t>
+  </si>
+  <si>
+    <t>Validation set used. For some reasons the validation losso continue to decrease</t>
   </si>
 </sst>
 </file>
@@ -231,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,7 +321,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7271,8 +7292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:S17"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63:E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7497,11 +7518,11 @@
     </row>
     <row r="5" spans="1:19" s="10" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -8141,11 +8162,11 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -8785,11 +8806,11 @@
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
@@ -9429,11 +9450,11 @@
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
@@ -10073,12 +10094,12 @@
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B63" s="25" t="s">
+      <c r="B63" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B64" s="11" t="s">
@@ -10367,11 +10388,11 @@
     </row>
     <row r="5" spans="1:19" s="10" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
@@ -10729,11 +10750,11 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
@@ -11088,11 +11109,11 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="15" t="s">
@@ -11447,11 +11468,11 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="s">
@@ -11806,10 +11827,10 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
+      <c r="B63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B64" s="11"/>
@@ -12271,11 +12292,11 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
@@ -12605,11 +12626,11 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
@@ -12939,11 +12960,11 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
@@ -13273,11 +13294,11 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
@@ -13607,10 +13628,10 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
+      <c r="B63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B64" s="11"/>
@@ -13928,7 +13949,7 @@
   <dimension ref="A1:S64"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:I29"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14032,11 +14053,11 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
@@ -14386,11 +14407,11 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
@@ -14740,11 +14761,11 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="19" t="s">
@@ -15094,11 +15115,11 @@
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="19" t="s">
@@ -15448,10 +15469,10 @@
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
+      <c r="B63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B64" s="11"/>
@@ -15764,8 +15785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C590A2-E27F-48E2-82ED-3E5DCC9A3C2D}">
   <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49:D57"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15825,7 +15846,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>11</v>
@@ -15864,16 +15885,24 @@
       </c>
     </row>
     <row r="5" spans="1:19" s="10" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="10" t="s">
-        <v>26</v>
+      <c r="D5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
@@ -15892,14 +15921,23 @@
       </c>
       <c r="B8" s="3">
         <f>AVERAGE(D8:AJ8)</f>
-        <v>0.69444399999999995</v>
+        <v>0.76388900000000004</v>
       </c>
       <c r="C8" s="4">
         <f>MAX(D8:AJ8)</f>
-        <v>0.69444399999999995</v>
+        <v>0.83680600000000005</v>
       </c>
       <c r="D8" s="23">
         <v>0.69444399999999995</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0.83680600000000005</v>
+      </c>
+      <c r="F8" s="24">
+        <v>0.71180600000000005</v>
+      </c>
+      <c r="G8" s="24">
+        <v>0.8125</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
@@ -15908,14 +15946,23 @@
       </c>
       <c r="B9" s="5">
         <f t="shared" ref="B9:B16" si="0">AVERAGE(D9:AJ9)</f>
-        <v>0.35763899999999998</v>
+        <v>0.48611124999999999</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" ref="C9:C16" si="1">MAX(D9:AJ9)</f>
-        <v>0.35763899999999998</v>
+        <v>0.60416700000000001</v>
       </c>
       <c r="D9" s="23">
         <v>0.35763899999999998</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0.60416700000000001</v>
+      </c>
+      <c r="F9" s="24">
+        <v>0.51041700000000001</v>
+      </c>
+      <c r="G9" s="24">
+        <v>0.47222199999999998</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -15924,14 +15971,23 @@
       </c>
       <c r="B10" s="5">
         <f t="shared" si="0"/>
-        <v>0.85069399999999995</v>
+        <v>0.88541650000000005</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="1"/>
-        <v>0.85069399999999995</v>
+        <v>0.9375</v>
       </c>
       <c r="D10" s="23">
         <v>0.85069399999999995</v>
+      </c>
+      <c r="E10" s="24">
+        <v>0.85763900000000004</v>
+      </c>
+      <c r="F10" s="24">
+        <v>0.89583299999999999</v>
+      </c>
+      <c r="G10" s="24">
+        <v>0.9375</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -15940,14 +15996,23 @@
       </c>
       <c r="B11" s="5">
         <f t="shared" si="0"/>
-        <v>0.52604200000000001</v>
+        <v>0.55598950000000003</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="1"/>
-        <v>0.52604200000000001</v>
+        <v>0.58333299999999999</v>
       </c>
       <c r="D11" s="23">
         <v>0.52604200000000001</v>
+      </c>
+      <c r="E11" s="24">
+        <v>0.546875</v>
+      </c>
+      <c r="F11" s="24">
+        <v>0.56770799999999999</v>
+      </c>
+      <c r="G11" s="24">
+        <v>0.58333299999999999</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -15956,14 +16021,23 @@
       </c>
       <c r="B12" s="5">
         <f t="shared" si="0"/>
-        <v>0.69444399999999995</v>
+        <v>0.67795124999999989</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="1"/>
-        <v>0.69444399999999995</v>
+        <v>0.72569399999999995</v>
       </c>
       <c r="D12" s="23">
         <v>0.69444399999999995</v>
+      </c>
+      <c r="E12" s="24">
+        <v>0.72569399999999995</v>
+      </c>
+      <c r="F12" s="24">
+        <v>0.65625</v>
+      </c>
+      <c r="G12" s="24">
+        <v>0.63541700000000001</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -15972,14 +16046,23 @@
       </c>
       <c r="B13" s="5">
         <f t="shared" si="0"/>
-        <v>0.79166700000000001</v>
+        <v>0.81857625000000001</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="1"/>
-        <v>0.79166700000000001</v>
+        <v>0.83333299999999999</v>
       </c>
       <c r="D13" s="23">
         <v>0.79166700000000001</v>
+      </c>
+      <c r="E13" s="24">
+        <v>0.81597200000000003</v>
+      </c>
+      <c r="F13" s="24">
+        <v>0.83333299999999999</v>
+      </c>
+      <c r="G13" s="24">
+        <v>0.83333299999999999</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -15988,14 +16071,23 @@
       </c>
       <c r="B14" s="5">
         <f t="shared" si="0"/>
-        <v>0.60763900000000004</v>
+        <v>0.69097200000000003</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="1"/>
-        <v>0.60763900000000004</v>
+        <v>0.77083299999999999</v>
       </c>
       <c r="D14" s="23">
         <v>0.60763900000000004</v>
+      </c>
+      <c r="E14" s="24">
+        <v>0.77083299999999999</v>
+      </c>
+      <c r="F14" s="24">
+        <v>0.61458299999999999</v>
+      </c>
+      <c r="G14" s="24">
+        <v>0.77083299999999999</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
@@ -16004,14 +16096,23 @@
       </c>
       <c r="B15" s="5">
         <f t="shared" si="0"/>
-        <v>0.80555600000000005</v>
+        <v>0.86111124999999999</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="1"/>
-        <v>0.80555600000000005</v>
+        <v>0.90277799999999997</v>
       </c>
       <c r="D15" s="23">
         <v>0.80555600000000005</v>
+      </c>
+      <c r="E15" s="24">
+        <v>0.85763900000000004</v>
+      </c>
+      <c r="F15" s="24">
+        <v>0.87847200000000003</v>
+      </c>
+      <c r="G15" s="24">
+        <v>0.90277799999999997</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -16020,14 +16121,23 @@
       </c>
       <c r="B16" s="7">
         <f t="shared" si="0"/>
-        <v>0.85416700000000001</v>
+        <v>0.88802100000000006</v>
       </c>
       <c r="C16" s="8">
         <f t="shared" si="1"/>
-        <v>0.85416700000000001</v>
+        <v>0.90277799999999997</v>
       </c>
       <c r="D16" s="23">
         <v>0.85416700000000001</v>
+      </c>
+      <c r="E16" s="24">
+        <v>0.89583299999999999</v>
+      </c>
+      <c r="F16" s="24">
+        <v>0.89930600000000005</v>
+      </c>
+      <c r="G16" s="24">
+        <v>0.90277799999999997</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -16036,27 +16146,27 @@
       </c>
       <c r="B17" s="22">
         <f>AVERAGE(B8:B16)</f>
-        <v>0.68692133333333338</v>
+        <v>0.73644866666666664</v>
       </c>
       <c r="C17" s="22">
         <f>AVERAGE(C8:C16)</f>
-        <v>0.68692133333333338</v>
+        <v>0.78858022222222202</v>
       </c>
       <c r="D17" s="22">
         <f t="shared" ref="D17:N17" si="2">AVERAGE(D8:D16)</f>
         <v>0.68692133333333338</v>
       </c>
-      <c r="E17" s="22" t="e">
+      <c r="E17" s="22">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="22" t="e">
+        <v>0.76793977777777778</v>
+      </c>
+      <c r="F17" s="22">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G17" s="22" t="e">
+        <v>0.72974533333333336</v>
+      </c>
+      <c r="G17" s="22">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.76118822222222216</v>
       </c>
       <c r="H17" s="22" t="e">
         <f t="shared" si="2"/>
@@ -16088,11 +16198,11 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
@@ -16111,14 +16221,23 @@
       </c>
       <c r="B21" s="3">
         <f>AVERAGE(D21:AJ21)</f>
-        <v>0.59259300000000004</v>
+        <v>0.68518524999999997</v>
       </c>
       <c r="C21" s="4">
         <f>MAX(D21:AJ21)</f>
-        <v>0.59259300000000004</v>
+        <v>0.78240699999999996</v>
       </c>
       <c r="D21" s="23">
         <v>0.59259300000000004</v>
+      </c>
+      <c r="E21" s="24">
+        <v>0.78240699999999996</v>
+      </c>
+      <c r="F21" s="24">
+        <v>0.61574099999999998</v>
+      </c>
+      <c r="G21" s="24">
+        <v>0.75</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -16127,14 +16246,23 @@
       </c>
       <c r="B22" s="5">
         <f t="shared" ref="B22:B29" si="3">AVERAGE(D22:AJ22)</f>
-        <v>0.14351900000000001</v>
+        <v>0.31481475000000003</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" ref="C22:C29" si="4">MAX(D22:AJ22)</f>
-        <v>0.14351900000000001</v>
+        <v>0.47222199999999998</v>
       </c>
       <c r="D22" s="23">
         <v>0.14351900000000001</v>
+      </c>
+      <c r="E22" s="24">
+        <v>0.47222199999999998</v>
+      </c>
+      <c r="F22" s="24">
+        <v>0.34722199999999998</v>
+      </c>
+      <c r="G22" s="24">
+        <v>0.296296</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -16143,14 +16271,23 @@
       </c>
       <c r="B23" s="5">
         <f t="shared" si="3"/>
-        <v>0.80092600000000003</v>
+        <v>0.84722225000000007</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="4"/>
-        <v>0.80092600000000003</v>
+        <v>0.91666700000000001</v>
       </c>
       <c r="D23" s="23">
         <v>0.80092600000000003</v>
+      </c>
+      <c r="E23" s="24">
+        <v>0.81018500000000004</v>
+      </c>
+      <c r="F23" s="24">
+        <v>0.86111099999999996</v>
+      </c>
+      <c r="G23" s="24">
+        <v>0.91666700000000001</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
@@ -16159,14 +16296,23 @@
       </c>
       <c r="B24" s="5">
         <f t="shared" si="3"/>
-        <v>0.36805599999999999</v>
+        <v>0.40798600000000002</v>
       </c>
       <c r="C24" s="6">
         <f t="shared" si="4"/>
-        <v>0.36805599999999999</v>
+        <v>0.44444400000000001</v>
       </c>
       <c r="D24" s="23">
         <v>0.36805599999999999</v>
+      </c>
+      <c r="E24" s="24">
+        <v>0.39583299999999999</v>
+      </c>
+      <c r="F24" s="24">
+        <v>0.42361100000000002</v>
+      </c>
+      <c r="G24" s="24">
+        <v>0.44444400000000001</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
@@ -16175,14 +16321,23 @@
       </c>
       <c r="B25" s="5">
         <f t="shared" si="3"/>
-        <v>0.59259300000000004</v>
+        <v>0.57060200000000005</v>
       </c>
       <c r="C25" s="6">
         <f t="shared" si="4"/>
-        <v>0.59259300000000004</v>
+        <v>0.63425900000000002</v>
       </c>
       <c r="D25" s="23">
         <v>0.59259300000000004</v>
+      </c>
+      <c r="E25" s="24">
+        <v>0.63425900000000002</v>
+      </c>
+      <c r="F25" s="24">
+        <v>0.54166700000000001</v>
+      </c>
+      <c r="G25" s="24">
+        <v>0.51388900000000004</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
@@ -16191,14 +16346,23 @@
       </c>
       <c r="B26" s="5">
         <f t="shared" si="3"/>
-        <v>0.72222200000000003</v>
+        <v>0.75810200000000005</v>
       </c>
       <c r="C26" s="6">
         <f t="shared" si="4"/>
-        <v>0.72222200000000003</v>
+        <v>0.77777799999999997</v>
       </c>
       <c r="D26" s="23">
         <v>0.72222200000000003</v>
+      </c>
+      <c r="E26" s="24">
+        <v>0.75463000000000002</v>
+      </c>
+      <c r="F26" s="24">
+        <v>0.77777799999999997</v>
+      </c>
+      <c r="G26" s="24">
+        <v>0.77777799999999997</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
@@ -16207,14 +16371,23 @@
       </c>
       <c r="B27" s="5">
         <f t="shared" si="3"/>
-        <v>0.476852</v>
+        <v>0.58796274999999998</v>
       </c>
       <c r="C27" s="6">
         <f t="shared" si="4"/>
-        <v>0.476852</v>
+        <v>0.69444399999999995</v>
       </c>
       <c r="D27" s="23">
         <v>0.476852</v>
+      </c>
+      <c r="E27" s="24">
+        <v>0.69444399999999995</v>
+      </c>
+      <c r="F27" s="24">
+        <v>0.48611100000000002</v>
+      </c>
+      <c r="G27" s="24">
+        <v>0.69444399999999995</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -16223,14 +16396,23 @@
       </c>
       <c r="B28" s="5">
         <f t="shared" si="3"/>
-        <v>0.74074099999999998</v>
+        <v>0.81481474999999992</v>
       </c>
       <c r="C28" s="6">
         <f t="shared" si="4"/>
-        <v>0.74074099999999998</v>
+        <v>0.87036999999999998</v>
       </c>
       <c r="D28" s="23">
         <v>0.74074099999999998</v>
+      </c>
+      <c r="E28" s="24">
+        <v>0.81018500000000004</v>
+      </c>
+      <c r="F28" s="24">
+        <v>0.83796300000000001</v>
+      </c>
+      <c r="G28" s="24">
+        <v>0.87036999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
@@ -16239,14 +16421,23 @@
       </c>
       <c r="B29" s="7">
         <f t="shared" si="3"/>
-        <v>0.80555600000000005</v>
+        <v>0.85069449999999991</v>
       </c>
       <c r="C29" s="8">
         <f t="shared" si="4"/>
-        <v>0.80555600000000005</v>
+        <v>0.87036999999999998</v>
       </c>
       <c r="D29" s="23">
         <v>0.80555600000000005</v>
+      </c>
+      <c r="E29" s="24">
+        <v>0.86111099999999996</v>
+      </c>
+      <c r="F29" s="24">
+        <v>0.86574099999999998</v>
+      </c>
+      <c r="G29" s="24">
+        <v>0.87036999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
@@ -16255,27 +16446,27 @@
       </c>
       <c r="B30" s="22">
         <f>AVERAGE(B21:B29)</f>
-        <v>0.58256200000000002</v>
+        <v>0.64859824999999993</v>
       </c>
       <c r="C30" s="22">
         <f>AVERAGE(C21:C29)</f>
-        <v>0.58256200000000002</v>
+        <v>0.71810677777777776</v>
       </c>
       <c r="D30" s="22">
         <f t="shared" ref="D30:N30" si="5">AVERAGE(D21:D29)</f>
         <v>0.58256200000000002</v>
       </c>
-      <c r="E30" s="22" t="e">
+      <c r="E30" s="22">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F30" s="22" t="e">
+        <v>0.69058622222222221</v>
+      </c>
+      <c r="F30" s="22">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G30" s="22" t="e">
+        <v>0.63966055555555557</v>
+      </c>
+      <c r="G30" s="22">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.68158422222222237</v>
       </c>
       <c r="H30" s="22" t="e">
         <f t="shared" si="5"/>
@@ -16307,11 +16498,11 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
@@ -16330,14 +16521,23 @@
       </c>
       <c r="B36" s="3">
         <f>AVERAGE(D36:AJ36)</f>
-        <v>0.74652799999999997</v>
+        <v>0.77690999999999999</v>
       </c>
       <c r="C36" s="4">
         <f>MAX(D36:AJ36)</f>
-        <v>0.74652799999999997</v>
+        <v>0.83680600000000005</v>
       </c>
       <c r="D36" s="23">
         <v>0.74652799999999997</v>
+      </c>
+      <c r="E36" s="24">
+        <v>0.83680600000000005</v>
+      </c>
+      <c r="F36" s="24">
+        <v>0.71180600000000005</v>
+      </c>
+      <c r="G36" s="24">
+        <v>0.8125</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
@@ -16346,14 +16546,23 @@
       </c>
       <c r="B37" s="5">
         <f t="shared" ref="B37:B44" si="6">AVERAGE(D37:AJ37)</f>
-        <v>0.48263899999999998</v>
+        <v>0.51736124999999999</v>
       </c>
       <c r="C37" s="6">
         <f t="shared" ref="C37:C44" si="7">MAX(D37:AJ37)</f>
-        <v>0.48263899999999998</v>
+        <v>0.60416700000000001</v>
       </c>
       <c r="D37" s="23">
         <v>0.48263899999999998</v>
+      </c>
+      <c r="E37" s="24">
+        <v>0.60416700000000001</v>
+      </c>
+      <c r="F37" s="24">
+        <v>0.51041700000000001</v>
+      </c>
+      <c r="G37" s="24">
+        <v>0.47222199999999998</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
@@ -16362,14 +16571,23 @@
       </c>
       <c r="B38" s="5">
         <f t="shared" si="6"/>
-        <v>0.875</v>
+        <v>0.89149299999999998</v>
       </c>
       <c r="C38" s="6">
         <f t="shared" si="7"/>
-        <v>0.875</v>
+        <v>0.9375</v>
       </c>
       <c r="D38" s="23">
         <v>0.875</v>
+      </c>
+      <c r="E38" s="24">
+        <v>0.85763900000000004</v>
+      </c>
+      <c r="F38" s="24">
+        <v>0.89583299999999999</v>
+      </c>
+      <c r="G38" s="24">
+        <v>0.9375</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
@@ -16378,14 +16596,23 @@
       </c>
       <c r="B39" s="5">
         <f t="shared" si="6"/>
-        <v>0.47395799999999999</v>
+        <v>0.54296850000000008</v>
       </c>
       <c r="C39" s="6">
         <f t="shared" si="7"/>
-        <v>0.47395799999999999</v>
+        <v>0.58333299999999999</v>
       </c>
       <c r="D39" s="23">
         <v>0.47395799999999999</v>
+      </c>
+      <c r="E39" s="24">
+        <v>0.546875</v>
+      </c>
+      <c r="F39" s="24">
+        <v>0.56770799999999999</v>
+      </c>
+      <c r="G39" s="24">
+        <v>0.58333299999999999</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
@@ -16394,7 +16621,7 @@
       </c>
       <c r="B40" s="5">
         <f t="shared" si="6"/>
-        <v>0.73611099999999996</v>
+        <v>0.68836799999999998</v>
       </c>
       <c r="C40" s="6">
         <f t="shared" si="7"/>
@@ -16403,6 +16630,15 @@
       <c r="D40" s="23">
         <v>0.73611099999999996</v>
       </c>
+      <c r="E40" s="24">
+        <v>0.72569399999999995</v>
+      </c>
+      <c r="F40" s="24">
+        <v>0.65625</v>
+      </c>
+      <c r="G40" s="24">
+        <v>0.63541700000000001</v>
+      </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="22">
@@ -16410,14 +16646,23 @@
       </c>
       <c r="B41" s="5">
         <f t="shared" si="6"/>
-        <v>0.77083299999999999</v>
+        <v>0.81336775000000006</v>
       </c>
       <c r="C41" s="6">
         <f t="shared" si="7"/>
-        <v>0.77083299999999999</v>
+        <v>0.83333299999999999</v>
       </c>
       <c r="D41" s="23">
         <v>0.77083299999999999</v>
+      </c>
+      <c r="E41" s="24">
+        <v>0.81597200000000003</v>
+      </c>
+      <c r="F41" s="24">
+        <v>0.83333299999999999</v>
+      </c>
+      <c r="G41" s="24">
+        <v>0.83333299999999999</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
@@ -16426,14 +16671,23 @@
       </c>
       <c r="B42" s="5">
         <f t="shared" si="6"/>
-        <v>0.69444399999999995</v>
+        <v>0.71267325000000004</v>
       </c>
       <c r="C42" s="6">
         <f t="shared" si="7"/>
-        <v>0.69444399999999995</v>
+        <v>0.77083299999999999</v>
       </c>
       <c r="D42" s="23">
         <v>0.69444399999999995</v>
+      </c>
+      <c r="E42" s="24">
+        <v>0.77083299999999999</v>
+      </c>
+      <c r="F42" s="24">
+        <v>0.61458299999999999</v>
+      </c>
+      <c r="G42" s="24">
+        <v>0.77083299999999999</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
@@ -16442,14 +16696,23 @@
       </c>
       <c r="B43" s="5">
         <f t="shared" si="6"/>
-        <v>0.82638900000000004</v>
+        <v>0.86631950000000002</v>
       </c>
       <c r="C43" s="6">
         <f t="shared" si="7"/>
-        <v>0.82638900000000004</v>
+        <v>0.90277799999999997</v>
       </c>
       <c r="D43" s="23">
         <v>0.82638900000000004</v>
+      </c>
+      <c r="E43" s="24">
+        <v>0.85763900000000004</v>
+      </c>
+      <c r="F43" s="24">
+        <v>0.87847200000000003</v>
+      </c>
+      <c r="G43" s="24">
+        <v>0.90277799999999997</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
@@ -16458,14 +16721,23 @@
       </c>
       <c r="B44" s="7">
         <f t="shared" si="6"/>
-        <v>0.875</v>
+        <v>0.89322925000000009</v>
       </c>
       <c r="C44" s="8">
         <f t="shared" si="7"/>
-        <v>0.875</v>
+        <v>0.90277799999999997</v>
       </c>
       <c r="D44" s="23">
         <v>0.875</v>
+      </c>
+      <c r="E44" s="24">
+        <v>0.89583299999999999</v>
+      </c>
+      <c r="F44" s="24">
+        <v>0.89930600000000005</v>
+      </c>
+      <c r="G44" s="24">
+        <v>0.90277799999999997</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
@@ -16474,27 +16746,27 @@
       </c>
       <c r="B45" s="22">
         <f>AVERAGE(B36:B44)</f>
-        <v>0.72010022222222214</v>
+        <v>0.74474338888888902</v>
       </c>
       <c r="C45" s="22">
         <f>AVERAGE(C36:C44)</f>
-        <v>0.72010022222222214</v>
+        <v>0.78973766666666656</v>
       </c>
       <c r="D45" s="22">
         <f t="shared" ref="D45:N45" si="8">AVERAGE(D36:D44)</f>
         <v>0.72010022222222214</v>
       </c>
-      <c r="E45" s="22" t="e">
+      <c r="E45" s="22">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F45" s="22" t="e">
+        <v>0.76793977777777778</v>
+      </c>
+      <c r="F45" s="22">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G45" s="22" t="e">
+        <v>0.72974533333333336</v>
+      </c>
+      <c r="G45" s="22">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>0.76118822222222216</v>
       </c>
       <c r="H45" s="22" t="e">
         <f t="shared" si="8"/>
@@ -16526,11 +16798,11 @@
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="22" t="s">
@@ -16549,14 +16821,23 @@
       </c>
       <c r="B49" s="3">
         <f>AVERAGE(D49:AJ49)</f>
-        <v>0.66203699999999999</v>
+        <v>0.70254624999999993</v>
       </c>
       <c r="C49" s="4">
         <f>MAX(D49:AJ49)</f>
-        <v>0.66203699999999999</v>
+        <v>0.78240699999999996</v>
       </c>
       <c r="D49" s="23">
         <v>0.66203699999999999</v>
+      </c>
+      <c r="E49" s="24">
+        <v>0.78240699999999996</v>
+      </c>
+      <c r="F49" s="24">
+        <v>0.61574099999999998</v>
+      </c>
+      <c r="G49" s="24">
+        <v>0.75</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
@@ -16565,14 +16846,23 @@
       </c>
       <c r="B50" s="5">
         <f t="shared" ref="B50:B57" si="9">AVERAGE(D50:AJ50)</f>
-        <v>0.31018499999999999</v>
+        <v>0.35648124999999997</v>
       </c>
       <c r="C50" s="6">
         <f t="shared" ref="C50:C57" si="10">MAX(D50:AJ50)</f>
-        <v>0.31018499999999999</v>
+        <v>0.47222199999999998</v>
       </c>
       <c r="D50" s="23">
         <v>0.31018499999999999</v>
+      </c>
+      <c r="E50" s="24">
+        <v>0.47222199999999998</v>
+      </c>
+      <c r="F50" s="24">
+        <v>0.34722199999999998</v>
+      </c>
+      <c r="G50" s="24">
+        <v>0.296296</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
@@ -16581,14 +16871,23 @@
       </c>
       <c r="B51" s="5">
         <f t="shared" si="9"/>
-        <v>0.83333299999999999</v>
+        <v>0.85532399999999997</v>
       </c>
       <c r="C51" s="6">
         <f t="shared" si="10"/>
-        <v>0.83333299999999999</v>
+        <v>0.91666700000000001</v>
       </c>
       <c r="D51" s="23">
         <v>0.83333299999999999</v>
+      </c>
+      <c r="E51" s="24">
+        <v>0.81018500000000004</v>
+      </c>
+      <c r="F51" s="24">
+        <v>0.86111099999999996</v>
+      </c>
+      <c r="G51" s="24">
+        <v>0.91666700000000001</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
@@ -16597,14 +16896,23 @@
       </c>
       <c r="B52" s="5">
         <f t="shared" si="9"/>
-        <v>0.29861100000000002</v>
+        <v>0.39062475000000002</v>
       </c>
       <c r="C52" s="6">
         <f t="shared" si="10"/>
-        <v>0.29861100000000002</v>
+        <v>0.44444400000000001</v>
       </c>
       <c r="D52" s="23">
         <v>0.29861100000000002</v>
+      </c>
+      <c r="E52" s="24">
+        <v>0.39583299999999999</v>
+      </c>
+      <c r="F52" s="24">
+        <v>0.42361100000000002</v>
+      </c>
+      <c r="G52" s="24">
+        <v>0.44444400000000001</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.3">
@@ -16613,7 +16921,7 @@
       </c>
       <c r="B53" s="5">
         <f t="shared" si="9"/>
-        <v>0.64814799999999995</v>
+        <v>0.58449075000000006</v>
       </c>
       <c r="C53" s="6">
         <f t="shared" si="10"/>
@@ -16622,6 +16930,15 @@
       <c r="D53" s="23">
         <v>0.64814799999999995</v>
       </c>
+      <c r="E53" s="24">
+        <v>0.63425900000000002</v>
+      </c>
+      <c r="F53" s="24">
+        <v>0.54166700000000001</v>
+      </c>
+      <c r="G53" s="24">
+        <v>0.51388900000000004</v>
+      </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="22">
@@ -16629,14 +16946,23 @@
       </c>
       <c r="B54" s="5">
         <f t="shared" si="9"/>
-        <v>0.69444399999999995</v>
+        <v>0.75115750000000003</v>
       </c>
       <c r="C54" s="6">
         <f t="shared" si="10"/>
-        <v>0.69444399999999995</v>
+        <v>0.77777799999999997</v>
       </c>
       <c r="D54" s="23">
         <v>0.69444399999999995</v>
+      </c>
+      <c r="E54" s="24">
+        <v>0.75463000000000002</v>
+      </c>
+      <c r="F54" s="24">
+        <v>0.77777799999999997</v>
+      </c>
+      <c r="G54" s="24">
+        <v>0.77777799999999997</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.3">
@@ -16645,14 +16971,23 @@
       </c>
       <c r="B55" s="5">
         <f t="shared" si="9"/>
-        <v>0.59259300000000004</v>
+        <v>0.61689799999999995</v>
       </c>
       <c r="C55" s="6">
         <f t="shared" si="10"/>
-        <v>0.59259300000000004</v>
+        <v>0.69444399999999995</v>
       </c>
       <c r="D55" s="23">
         <v>0.59259300000000004</v>
+      </c>
+      <c r="E55" s="24">
+        <v>0.69444399999999995</v>
+      </c>
+      <c r="F55" s="24">
+        <v>0.48611100000000002</v>
+      </c>
+      <c r="G55" s="24">
+        <v>0.69444399999999995</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
@@ -16661,14 +16996,23 @@
       </c>
       <c r="B56" s="5">
         <f t="shared" si="9"/>
-        <v>0.76851899999999995</v>
+        <v>0.82175925000000005</v>
       </c>
       <c r="C56" s="6">
         <f t="shared" si="10"/>
-        <v>0.76851899999999995</v>
+        <v>0.87036999999999998</v>
       </c>
       <c r="D56" s="23">
         <v>0.76851899999999995</v>
+      </c>
+      <c r="E56" s="24">
+        <v>0.81018500000000004</v>
+      </c>
+      <c r="F56" s="24">
+        <v>0.83796300000000001</v>
+      </c>
+      <c r="G56" s="24">
+        <v>0.87036999999999998</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
@@ -16677,14 +17021,23 @@
       </c>
       <c r="B57" s="7">
         <f t="shared" si="9"/>
-        <v>0.83333299999999999</v>
+        <v>0.85763874999999989</v>
       </c>
       <c r="C57" s="8">
         <f t="shared" si="10"/>
-        <v>0.83333299999999999</v>
+        <v>0.87036999999999998</v>
       </c>
       <c r="D57" s="23">
         <v>0.83333299999999999</v>
+      </c>
+      <c r="E57" s="24">
+        <v>0.86111099999999996</v>
+      </c>
+      <c r="F57" s="24">
+        <v>0.86574099999999998</v>
+      </c>
+      <c r="G57" s="24">
+        <v>0.87036999999999998</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.3">
@@ -16693,27 +17046,27 @@
       </c>
       <c r="B58" s="22">
         <f>AVERAGE(B49:B57)</f>
-        <v>0.62680033333333318</v>
+        <v>0.65965783333333339</v>
       </c>
       <c r="C58" s="22">
         <f>AVERAGE(C49:C57)</f>
-        <v>0.62680033333333318</v>
+        <v>0.71965000000000001</v>
       </c>
       <c r="D58" s="22">
         <f t="shared" ref="D58:N58" si="11">AVERAGE(D49:D57)</f>
         <v>0.62680033333333318</v>
       </c>
-      <c r="E58" s="22" t="e">
+      <c r="E58" s="22">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F58" s="22" t="e">
+        <v>0.69058622222222221</v>
+      </c>
+      <c r="F58" s="22">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G58" s="22" t="e">
+        <v>0.63966055555555557</v>
+      </c>
+      <c r="G58" s="22">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0.68158422222222237</v>
       </c>
       <c r="H58" s="22" t="e">
         <f t="shared" si="11"/>
@@ -16745,16 +17098,24 @@
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
+      <c r="B63" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B64" s="11"/>
+      <c r="B64" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C64" s="24"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A34:C34"/>

</xml_diff>